<commit_message>
Updated docs for 0.2.0
</commit_message>
<xml_diff>
--- a/inst/extdata/fluctest_template.xlsx
+++ b/inst/extdata/fluctest_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git repositories\pseudonoma\luria\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535784E6-6EDC-46E8-BA4D-86D18E94EC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAF67CF-ED14-4948-89ED-D53825B42521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D17F2159-7E7C-4C2C-8D2E-612E10CB3E15}"/>
+    <workbookView xWindow="0" yWindow="1425" windowWidth="28800" windowHeight="14175" xr2:uid="{D17F2159-7E7C-4C2C-8D2E-612E10CB3E15}"/>
   </bookViews>
   <sheets>
     <sheet name="Example layout" sheetId="1" r:id="rId1"/>
@@ -480,9 +480,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -520,7 +520,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -626,7 +626,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -768,7 +768,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -778,7 +778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CCF9C36-DE6B-4F3E-8A95-159558DCECAA}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1596,9 +1596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C6956AB-B23C-4D71-9BCB-01FF4CAA0BA2}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>